<commit_message>
UPDATE: Clustering and Useless columns
</commit_message>
<xml_diff>
--- a/correlation_matrix.xlsx
+++ b/correlation_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,90 +533,80 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>domestic gross ($million)</t>
+          <t>worldwide gross</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1066897969101734</v>
+        <v>0.105525492718214</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>worldwide gross</t>
+          <t>of gross earned abroad</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.105525492718214</v>
+        <v>0.1024831696413194</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>of gross earned abroad</t>
+          <t>foreign gross</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1024831696413194</v>
+        <v>0.09679870169545644</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>foreign gross</t>
+          <t>worldwide gross ($million)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.09679870169545644</v>
+        <v>0.09532295012105929</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>worldwide gross ($million)</t>
+          <t>imdb rating</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09532295012105929</v>
+        <v>0.09216721772651079</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>imdb rating</t>
+          <t>rotten tomatoes vs metacritic deviance</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.09216721772651079</v>
+        <v>0.09090856420798747</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>rotten tomatoes vs metacritic deviance</t>
+          <t>foreign gross ($million)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.09090856420798747</v>
+        <v>0.02830693191420764</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>foreign gross ($million)</t>
+          <t>opening weekend ($million)</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.02830693191420764</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>opening weekend ($million)</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
         <v>0.004981924126467788</v>
       </c>
     </row>

</xml_diff>